<commit_message>
added behavioral descriptive stats
</commit_message>
<xml_diff>
--- a/DataAnalysis/results/preprocessed.xlsx
+++ b/DataAnalysis/results/preprocessed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="86">
   <si>
     <t>case</t>
   </si>
@@ -37,6 +37,9 @@
     <t>correctness</t>
   </si>
   <si>
+    <t>Run Out Of Time</t>
+  </si>
+  <si>
     <t>Outlier</t>
   </si>
   <si>
@@ -79,9 +82,21 @@
     <t>Arooba</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>it searches for a given number (here: 10) in the array; in this case it will return 3 as position</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>Element not present</t>
   </si>
   <si>
@@ -124,6 +139,9 @@
     <t>{3,16,23,42,61,75,536}</t>
   </si>
   <si>
+    <t>nan</t>
+  </si>
+  <si>
     <t xml:space="preserve">it prints out the array as String but in a different order (smallest to </t>
   </si>
   <si>
@@ -133,9 +151,15 @@
     <t>536, 75, 61, 42, 23, 16, 3</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>it multiplies 3 times 2 times 1</t>
   </si>
   <si>
+    <t>120</t>
+  </si>
+  <si>
     <t>2 6 2120</t>
   </si>
   <si>
@@ -145,9 +169,15 @@
     <t xml:space="preserve">I recursivly calculates the Fibonacci(x) function, so it returns the n'th Fibonacci </t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>'0100001</t>
   </si>
   <si>
+    <t>10001</t>
+  </si>
+  <si>
     <t xml:space="preserve">4 -&gt; 2 -&gt; </t>
   </si>
   <si>
@@ -157,6 +187,9 @@
     <t xml:space="preserve">0, 2, 4 </t>
   </si>
   <si>
+    <t>1000</t>
+  </si>
+  <si>
     <t xml:space="preserve">it print the number 17 in binary -&gt; with mod 2 and the leftover again to fill the binaryNum list </t>
   </si>
   <si>
@@ -202,6 +235,9 @@
     <t>6 6 6 12 12 12 18 18 18</t>
   </si>
   <si>
+    <t>15</t>
+  </si>
+  <si>
     <t>calculate the prime factors  using modulo and print it out</t>
   </si>
   <si>
@@ -233,6 +269,9 @@
   </si>
   <si>
     <t>"gnikcarTeyE"</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -590,13 +629,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H158"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,19 +660,22 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>198</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -647,19 +689,22 @@
       <c r="H2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>211</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -673,19 +718,22 @@
       <c r="H3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>224</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -699,19 +747,22 @@
       <c r="H4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>231</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -725,19 +776,22 @@
       <c r="H5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>232</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -751,19 +805,22 @@
       <c r="H6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>235</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -777,19 +834,22 @@
       <c r="H7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>240</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -803,19 +863,22 @@
       <c r="H8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>165</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -829,19 +892,22 @@
       <c r="H9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>206</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -853,21 +919,24 @@
         <v>0</v>
       </c>
       <c r="H10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>214</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -881,19 +950,22 @@
       <c r="H11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>230</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -907,19 +979,22 @@
       <c r="H12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>238</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -933,19 +1008,22 @@
       <c r="H13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>182</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -959,19 +1037,22 @@
       <c r="H14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>210</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -985,19 +1066,22 @@
       <c r="H15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>212</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1011,19 +1095,22 @@
       <c r="H16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>226</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -1037,19 +1124,22 @@
       <c r="H17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>234</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -1063,19 +1153,22 @@
       <c r="H18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>175</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -1089,19 +1182,22 @@
       <c r="H19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>209</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -1115,19 +1211,22 @@
       <c r="H20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>222</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -1141,19 +1240,22 @@
       <c r="H21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>223</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -1167,19 +1269,22 @@
       <c r="H22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>236</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -1193,19 +1298,22 @@
       <c r="H23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>182</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -1219,19 +1327,22 @@
       <c r="H24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>210</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -1245,19 +1356,22 @@
       <c r="H25" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>212</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -1271,19 +1385,22 @@
       <c r="H26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>226</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -1297,19 +1414,22 @@
       <c r="H27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>234</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -1323,19 +1443,22 @@
       <c r="H28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>198</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -1349,19 +1472,22 @@
       <c r="H29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>211</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -1375,19 +1501,22 @@
       <c r="H30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>224</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D31" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
@@ -1401,19 +1530,22 @@
       <c r="H31" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>231</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -1427,19 +1559,22 @@
       <c r="H32" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>232</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -1453,19 +1588,22 @@
       <c r="H33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>235</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -1479,19 +1617,22 @@
       <c r="H34" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>240</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -1505,19 +1646,22 @@
       <c r="H35" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>175</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D36" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -1531,19 +1675,22 @@
       <c r="H36" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>209</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -1557,19 +1704,22 @@
       <c r="H37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>222</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
@@ -1583,19 +1733,22 @@
       <c r="H38" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>223</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -1609,19 +1762,22 @@
       <c r="H39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>236</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D40" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
@@ -1635,16 +1791,22 @@
       <c r="H40" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>165</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="D41" t="s">
+        <v>41</v>
       </c>
       <c r="E41" t="b">
         <v>1</v>
@@ -1656,21 +1818,24 @@
         <v>0</v>
       </c>
       <c r="H41" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>206</v>
       </c>
       <c r="B42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
+        <v>24</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -1682,21 +1847,24 @@
         <v>0</v>
       </c>
       <c r="H42" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>214</v>
       </c>
       <c r="B43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -1710,19 +1878,22 @@
       <c r="H43" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>230</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D44" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
@@ -1736,19 +1907,22 @@
       <c r="H44" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>238</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D45" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E45" t="b">
         <v>0</v>
@@ -1762,16 +1936,22 @@
       <c r="H45" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="I45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>175</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D46" t="s">
+        <v>41</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
@@ -1785,19 +1965,22 @@
       <c r="H46" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47">
         <v>182</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
@@ -1811,16 +1994,22 @@
       <c r="H47" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48">
         <v>210</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D48" t="s">
+        <v>41</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -1834,19 +2023,22 @@
       <c r="H48" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="I48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49">
         <v>212</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="D49" t="s">
+        <v>45</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -1860,19 +2052,22 @@
       <c r="H49" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="I49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50">
         <v>226</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="D50" t="s">
+        <v>45</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -1886,19 +2081,22 @@
       <c r="H50" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51">
         <v>234</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="D51" t="s">
+        <v>45</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -1912,16 +2110,22 @@
       <c r="H51" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="I51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52">
         <v>165</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C52" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D52" t="s">
+        <v>41</v>
       </c>
       <c r="E52" t="b">
         <v>1</v>
@@ -1933,21 +2137,24 @@
         <v>0</v>
       </c>
       <c r="H52" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53">
         <v>206</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>14</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="D53" t="s">
+        <v>24</v>
       </c>
       <c r="E53" t="b">
         <v>0</v>
@@ -1959,21 +2166,24 @@
         <v>0</v>
       </c>
       <c r="H53" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54">
         <v>214</v>
       </c>
       <c r="B54" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
@@ -1987,19 +2197,22 @@
       <c r="H54" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:8">
+      <c r="I54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55">
         <v>230</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C55" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="D55" t="s">
+        <v>45</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
@@ -2013,19 +2226,22 @@
       <c r="H55" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:8">
+      <c r="I55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56">
         <v>238</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C56" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="D56" t="s">
+        <v>45</v>
       </c>
       <c r="E56" t="b">
         <v>0</v>
@@ -2039,19 +2255,22 @@
       <c r="H56" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="I56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57">
         <v>198</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C57" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D57" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E57" t="b">
         <v>0</v>
@@ -2065,16 +2284,22 @@
       <c r="H57" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:8">
+      <c r="I57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58">
         <v>211</v>
       </c>
       <c r="B58" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D58" t="s">
+        <v>41</v>
       </c>
       <c r="E58" t="b">
         <v>0</v>
@@ -2088,19 +2313,22 @@
       <c r="H58" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="I58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59">
         <v>224</v>
       </c>
       <c r="B59" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59">
-        <v>120</v>
+        <v>15</v>
+      </c>
+      <c r="D59" t="s">
+        <v>47</v>
       </c>
       <c r="E59" t="b">
         <v>0</v>
@@ -2114,19 +2342,22 @@
       <c r="H59" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="I59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60">
         <v>231</v>
       </c>
       <c r="B60" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60">
-        <v>120</v>
+        <v>15</v>
+      </c>
+      <c r="D60" t="s">
+        <v>47</v>
       </c>
       <c r="E60" t="b">
         <v>0</v>
@@ -2140,19 +2371,22 @@
       <c r="H60" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:8">
+      <c r="I60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61">
         <v>232</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C61" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61">
-        <v>120</v>
+        <v>15</v>
+      </c>
+      <c r="D61" t="s">
+        <v>47</v>
       </c>
       <c r="E61" t="b">
         <v>0</v>
@@ -2166,19 +2400,22 @@
       <c r="H61" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:8">
+      <c r="I61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62">
         <v>235</v>
       </c>
       <c r="B62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D62" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E62" t="b">
         <v>0</v>
@@ -2192,19 +2429,22 @@
       <c r="H62" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="I62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63">
         <v>240</v>
       </c>
       <c r="B63" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C63" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63">
-        <v>120</v>
+        <v>15</v>
+      </c>
+      <c r="D63" t="s">
+        <v>47</v>
       </c>
       <c r="E63" t="b">
         <v>0</v>
@@ -2218,16 +2458,22 @@
       <c r="H63" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="I63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64">
         <v>165</v>
       </c>
       <c r="B64" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="D64" t="s">
+        <v>41</v>
       </c>
       <c r="E64" t="b">
         <v>1</v>
@@ -2239,21 +2485,24 @@
         <v>0</v>
       </c>
       <c r="H64" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65">
         <v>206</v>
       </c>
       <c r="B65" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>15</v>
-      </c>
-      <c r="D65">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="D65" t="s">
+        <v>24</v>
       </c>
       <c r="E65" t="b">
         <v>0</v>
@@ -2265,21 +2514,24 @@
         <v>0</v>
       </c>
       <c r="H65" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66">
         <v>214</v>
       </c>
       <c r="B66" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D66" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E66" t="b">
         <v>0</v>
@@ -2293,19 +2545,22 @@
       <c r="H66" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="I66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67">
         <v>230</v>
       </c>
       <c r="B67" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>15</v>
-      </c>
-      <c r="D67">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="D67" t="s">
+        <v>23</v>
       </c>
       <c r="E67" t="b">
         <v>0</v>
@@ -2319,19 +2574,22 @@
       <c r="H67" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:8">
+      <c r="I67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68">
         <v>238</v>
       </c>
       <c r="B68" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>15</v>
-      </c>
-      <c r="D68">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="D68" t="s">
+        <v>26</v>
       </c>
       <c r="E68" t="b">
         <v>0</v>
@@ -2345,19 +2603,22 @@
       <c r="H68" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="I68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69">
         <v>175</v>
       </c>
       <c r="B69" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C69" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D69" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E69" t="b">
         <v>0</v>
@@ -2371,19 +2632,22 @@
       <c r="H69" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:8">
+      <c r="I69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70">
         <v>209</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C70" t="s">
-        <v>15</v>
-      </c>
-      <c r="D70">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="D70" t="s">
+        <v>22</v>
       </c>
       <c r="E70" t="b">
         <v>0</v>
@@ -2397,19 +2661,22 @@
       <c r="H70" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:8">
+      <c r="I70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71">
         <v>222</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C71" t="s">
-        <v>15</v>
-      </c>
-      <c r="D71">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="D71" t="s">
+        <v>22</v>
       </c>
       <c r="E71" t="b">
         <v>0</v>
@@ -2423,19 +2690,22 @@
       <c r="H71" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:8">
+      <c r="I71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72">
         <v>223</v>
       </c>
       <c r="B72" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C72" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D72" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E72" t="b">
         <v>0</v>
@@ -2449,19 +2719,22 @@
       <c r="H72" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:8">
+      <c r="I72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73">
         <v>236</v>
       </c>
       <c r="B73" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C73" t="s">
-        <v>15</v>
-      </c>
-      <c r="D73">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="D73" t="s">
+        <v>22</v>
       </c>
       <c r="E73" t="b">
         <v>0</v>
@@ -2475,16 +2748,22 @@
       <c r="H73" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:8">
+      <c r="I73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74">
         <v>198</v>
       </c>
       <c r="B74" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C74" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="D74" t="s">
+        <v>41</v>
       </c>
       <c r="E74" t="b">
         <v>0</v>
@@ -2498,19 +2777,22 @@
       <c r="H74" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:8">
+      <c r="I74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75">
         <v>211</v>
       </c>
       <c r="B75" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C75" t="s">
-        <v>15</v>
-      </c>
-      <c r="D75">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="D75" t="s">
+        <v>22</v>
       </c>
       <c r="E75" t="b">
         <v>0</v>
@@ -2524,19 +2806,22 @@
       <c r="H75" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:8">
+      <c r="I75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76">
         <v>224</v>
       </c>
       <c r="B76" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C76" t="s">
-        <v>15</v>
-      </c>
-      <c r="D76">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="D76" t="s">
+        <v>23</v>
       </c>
       <c r="E76" t="b">
         <v>0</v>
@@ -2550,19 +2835,22 @@
       <c r="H76" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:8">
+      <c r="I76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77">
         <v>231</v>
       </c>
       <c r="B77" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C77" t="s">
-        <v>15</v>
-      </c>
-      <c r="D77">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="D77" t="s">
+        <v>23</v>
       </c>
       <c r="E77" t="b">
         <v>0</v>
@@ -2576,19 +2864,22 @@
       <c r="H77" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:8">
+      <c r="I77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78">
         <v>232</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C78" t="s">
-        <v>15</v>
-      </c>
-      <c r="D78">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="D78" t="s">
+        <v>23</v>
       </c>
       <c r="E78" t="b">
         <v>0</v>
@@ -2602,16 +2893,22 @@
       <c r="H78" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:8">
+      <c r="I78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
       <c r="A79">
         <v>235</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C79" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="D79" t="s">
+        <v>41</v>
       </c>
       <c r="E79" t="b">
         <v>0</v>
@@ -2625,19 +2922,22 @@
       <c r="H79" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:8">
+      <c r="I79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
       <c r="A80">
         <v>240</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C80" t="s">
-        <v>15</v>
-      </c>
-      <c r="D80">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="D80" t="s">
+        <v>23</v>
       </c>
       <c r="E80" t="b">
         <v>0</v>
@@ -2651,19 +2951,22 @@
       <c r="H80" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:8">
+      <c r="I80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
       <c r="A81">
         <v>182</v>
       </c>
       <c r="B81" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C81" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D81" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E81" t="b">
         <v>0</v>
@@ -2677,19 +2980,22 @@
       <c r="H81" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:8">
+      <c r="I81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
       <c r="A82">
         <v>210</v>
       </c>
       <c r="B82" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C82" t="s">
-        <v>15</v>
-      </c>
-      <c r="D82">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="D82" t="s">
+        <v>23</v>
       </c>
       <c r="E82" t="b">
         <v>0</v>
@@ -2703,16 +3009,22 @@
       <c r="H82" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:8">
+      <c r="I82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
       <c r="A83">
         <v>212</v>
       </c>
       <c r="B83" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="D83" t="s">
+        <v>41</v>
       </c>
       <c r="E83" t="b">
         <v>1</v>
@@ -2724,21 +3036,24 @@
         <v>0</v>
       </c>
       <c r="H83" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
       <c r="A84">
         <v>226</v>
       </c>
       <c r="B84" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C84" t="s">
-        <v>15</v>
-      </c>
-      <c r="D84">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="D84" t="s">
+        <v>51</v>
       </c>
       <c r="E84" t="b">
         <v>0</v>
@@ -2752,19 +3067,22 @@
       <c r="H84" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:8">
+      <c r="I84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
       <c r="A85">
         <v>234</v>
       </c>
       <c r="B85" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C85" t="s">
-        <v>15</v>
-      </c>
-      <c r="D85">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="D85" t="s">
+        <v>24</v>
       </c>
       <c r="E85" t="b">
         <v>0</v>
@@ -2778,19 +3096,22 @@
       <c r="H85" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:8">
+      <c r="I85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
       <c r="A86">
         <v>198</v>
       </c>
       <c r="B86" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D86" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E86" t="b">
         <v>0</v>
@@ -2804,19 +3125,22 @@
       <c r="H86" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:8">
+      <c r="I86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
       <c r="A87">
         <v>211</v>
       </c>
       <c r="B87" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C87" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D87" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E87" t="b">
         <v>0</v>
@@ -2830,19 +3154,22 @@
       <c r="H87" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:8">
+      <c r="I87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
       <c r="A88">
         <v>224</v>
       </c>
       <c r="B88" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C88" t="s">
-        <v>16</v>
-      </c>
-      <c r="D88">
-        <v>10001</v>
+        <v>17</v>
+      </c>
+      <c r="D88" t="s">
+        <v>53</v>
       </c>
       <c r="E88" t="b">
         <v>0</v>
@@ -2856,19 +3183,22 @@
       <c r="H88" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:8">
+      <c r="I88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
       <c r="A89">
         <v>231</v>
       </c>
       <c r="B89" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C89" t="s">
-        <v>16</v>
-      </c>
-      <c r="D89">
-        <v>10001</v>
+        <v>17</v>
+      </c>
+      <c r="D89" t="s">
+        <v>53</v>
       </c>
       <c r="E89" t="b">
         <v>0</v>
@@ -2882,19 +3212,22 @@
       <c r="H89" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:8">
+      <c r="I89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
       <c r="A90">
         <v>232</v>
       </c>
       <c r="B90" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C90" t="s">
-        <v>16</v>
-      </c>
-      <c r="D90">
-        <v>10001</v>
+        <v>17</v>
+      </c>
+      <c r="D90" t="s">
+        <v>53</v>
       </c>
       <c r="E90" t="b">
         <v>0</v>
@@ -2908,19 +3241,22 @@
       <c r="H90" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:8">
+      <c r="I90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
       <c r="A91">
         <v>235</v>
       </c>
       <c r="B91" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C91" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D91" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E91" t="b">
         <v>0</v>
@@ -2934,19 +3270,22 @@
       <c r="H91" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:8">
+      <c r="I91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
       <c r="A92">
         <v>240</v>
       </c>
       <c r="B92" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C92" t="s">
-        <v>16</v>
-      </c>
-      <c r="D92">
-        <v>10001</v>
+        <v>17</v>
+      </c>
+      <c r="D92" t="s">
+        <v>53</v>
       </c>
       <c r="E92" t="b">
         <v>0</v>
@@ -2960,16 +3299,22 @@
       <c r="H92" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:8">
+      <c r="I92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
       <c r="A93">
         <v>165</v>
       </c>
       <c r="B93" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C93" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D93" t="s">
+        <v>41</v>
       </c>
       <c r="E93" t="b">
         <v>1</v>
@@ -2981,21 +3326,24 @@
         <v>0</v>
       </c>
       <c r="H93" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
       <c r="A94">
         <v>206</v>
       </c>
       <c r="B94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C94" t="s">
-        <v>16</v>
-      </c>
-      <c r="D94">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="D94" t="s">
+        <v>24</v>
       </c>
       <c r="E94" t="b">
         <v>0</v>
@@ -3007,21 +3355,24 @@
         <v>0</v>
       </c>
       <c r="H94" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
       <c r="A95">
         <v>214</v>
       </c>
       <c r="B95" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C95" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D95" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E95" t="b">
         <v>0</v>
@@ -3035,19 +3386,22 @@
       <c r="H95" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:8">
+      <c r="I95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
       <c r="A96">
         <v>230</v>
       </c>
       <c r="B96" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C96" t="s">
-        <v>16</v>
-      </c>
-      <c r="D96">
-        <v>10001</v>
+        <v>17</v>
+      </c>
+      <c r="D96" t="s">
+        <v>53</v>
       </c>
       <c r="E96" t="b">
         <v>0</v>
@@ -3061,19 +3415,22 @@
       <c r="H96" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:8">
+      <c r="I96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
       <c r="A97">
         <v>238</v>
       </c>
       <c r="B97" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C97" t="s">
-        <v>16</v>
-      </c>
-      <c r="D97">
-        <v>10001</v>
+        <v>17</v>
+      </c>
+      <c r="D97" t="s">
+        <v>53</v>
       </c>
       <c r="E97" t="b">
         <v>0</v>
@@ -3087,19 +3444,22 @@
       <c r="H97" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:8">
+      <c r="I97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
       <c r="A98">
         <v>182</v>
       </c>
       <c r="B98" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C98" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D98" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E98" t="b">
         <v>0</v>
@@ -3113,19 +3473,22 @@
       <c r="H98" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:8">
+      <c r="I98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
       <c r="A99">
         <v>210</v>
       </c>
       <c r="B99" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C99" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D99" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="E99" t="b">
         <v>0</v>
@@ -3139,16 +3502,22 @@
       <c r="H99" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:8">
+      <c r="I99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
       <c r="A100">
         <v>212</v>
       </c>
       <c r="B100" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C100" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D100" t="s">
+        <v>41</v>
       </c>
       <c r="E100" t="b">
         <v>1</v>
@@ -3160,18 +3529,24 @@
         <v>0</v>
       </c>
       <c r="H100" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
       <c r="A101">
         <v>226</v>
       </c>
       <c r="B101" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C101" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D101" t="s">
+        <v>41</v>
       </c>
       <c r="E101" t="b">
         <v>1</v>
@@ -3183,21 +3558,24 @@
         <v>0</v>
       </c>
       <c r="H101" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
       <c r="A102">
         <v>234</v>
       </c>
       <c r="B102" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C102" t="s">
-        <v>16</v>
-      </c>
-      <c r="D102">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="D102" t="s">
+        <v>24</v>
       </c>
       <c r="E102" t="b">
         <v>0</v>
@@ -3211,16 +3589,22 @@
       <c r="H102" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:8">
+      <c r="I102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
       <c r="A103">
         <v>175</v>
       </c>
       <c r="B103" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D103" t="s">
+        <v>41</v>
       </c>
       <c r="E103" t="b">
         <v>1</v>
@@ -3232,21 +3616,24 @@
         <v>0</v>
       </c>
       <c r="H103" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I103" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
       <c r="A104">
         <v>209</v>
       </c>
       <c r="B104" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C104" t="s">
-        <v>16</v>
-      </c>
-      <c r="D104">
-        <v>10001</v>
+        <v>17</v>
+      </c>
+      <c r="D104" t="s">
+        <v>53</v>
       </c>
       <c r="E104" t="b">
         <v>0</v>
@@ -3260,19 +3647,22 @@
       <c r="H104" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:8">
+      <c r="I104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
       <c r="A105">
         <v>222</v>
       </c>
       <c r="B105" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C105" t="s">
-        <v>16</v>
-      </c>
-      <c r="D105">
-        <v>1000</v>
+        <v>17</v>
+      </c>
+      <c r="D105" t="s">
+        <v>57</v>
       </c>
       <c r="E105" t="b">
         <v>0</v>
@@ -3286,19 +3676,22 @@
       <c r="H105" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:8">
+      <c r="I105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
       <c r="A106">
         <v>223</v>
       </c>
       <c r="B106" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C106" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D106" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E106" t="b">
         <v>0</v>
@@ -3312,16 +3705,22 @@
       <c r="H106" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:8">
+      <c r="I106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
       <c r="A107">
         <v>236</v>
       </c>
       <c r="B107" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C107" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D107" t="s">
+        <v>41</v>
       </c>
       <c r="E107" t="b">
         <v>1</v>
@@ -3333,21 +3732,24 @@
         <v>0</v>
       </c>
       <c r="H107" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
       <c r="A108">
         <v>182</v>
       </c>
       <c r="B108" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C108" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D108" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E108" t="b">
         <v>0</v>
@@ -3361,19 +3763,22 @@
       <c r="H108" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:8">
+      <c r="I108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
       <c r="A109">
         <v>210</v>
       </c>
       <c r="B109" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C109" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D109" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E109" t="b">
         <v>0</v>
@@ -3387,16 +3792,22 @@
       <c r="H109" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:8">
+      <c r="I109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
       <c r="A110">
         <v>212</v>
       </c>
       <c r="B110" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C110" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D110" t="s">
+        <v>41</v>
       </c>
       <c r="E110" t="b">
         <v>1</v>
@@ -3408,21 +3819,24 @@
         <v>0</v>
       </c>
       <c r="H110" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
       <c r="A111">
         <v>226</v>
       </c>
       <c r="B111" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C111" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D111" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="E111" t="b">
         <v>0</v>
@@ -3436,19 +3850,22 @@
       <c r="H111" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:8">
+      <c r="I111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
       <c r="A112">
         <v>234</v>
       </c>
       <c r="B112" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C112" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D112" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E112" t="b">
         <v>0</v>
@@ -3462,19 +3879,22 @@
       <c r="H112" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:8">
+      <c r="I112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
       <c r="A113">
         <v>198</v>
       </c>
       <c r="B113" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C113" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D113" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E113" t="b">
         <v>0</v>
@@ -3488,19 +3908,22 @@
       <c r="H113" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:8">
+      <c r="I113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
       <c r="A114">
         <v>211</v>
       </c>
       <c r="B114" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C114" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D114" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E114" t="b">
         <v>0</v>
@@ -3514,19 +3937,22 @@
       <c r="H114" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:8">
+      <c r="I114" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
       <c r="A115">
         <v>224</v>
       </c>
       <c r="B115" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C115" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D115" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E115" t="b">
         <v>0</v>
@@ -3540,19 +3966,22 @@
       <c r="H115" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:8">
+      <c r="I115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
       <c r="A116">
         <v>231</v>
       </c>
       <c r="B116" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C116" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D116" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="E116" t="b">
         <v>0</v>
@@ -3566,19 +3995,22 @@
       <c r="H116" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:8">
+      <c r="I116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
       <c r="A117">
         <v>232</v>
       </c>
       <c r="B117" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C117" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D117" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E117" t="b">
         <v>0</v>
@@ -3592,16 +4024,22 @@
       <c r="H117" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:8">
+      <c r="I117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
       <c r="A118">
         <v>235</v>
       </c>
       <c r="B118" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C118" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D118" t="s">
+        <v>41</v>
       </c>
       <c r="E118" t="b">
         <v>0</v>
@@ -3615,19 +4053,22 @@
       <c r="H118" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:8">
+      <c r="I118" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
       <c r="A119">
         <v>240</v>
       </c>
       <c r="B119" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C119" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D119" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="E119" t="b">
         <v>0</v>
@@ -3641,19 +4082,22 @@
       <c r="H119" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:8">
+      <c r="I119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
       <c r="A120">
         <v>175</v>
       </c>
       <c r="B120" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C120" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D120" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E120" t="b">
         <v>0</v>
@@ -3667,19 +4111,22 @@
       <c r="H120" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:8">
+      <c r="I120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
       <c r="A121">
         <v>209</v>
       </c>
       <c r="B121" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C121" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D121" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="E121" t="b">
         <v>0</v>
@@ -3693,19 +4140,22 @@
       <c r="H121" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:8">
+      <c r="I121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
       <c r="A122">
         <v>222</v>
       </c>
       <c r="B122" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C122" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D122" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="E122" t="b">
         <v>0</v>
@@ -3719,19 +4169,22 @@
       <c r="H122" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:8">
+      <c r="I122" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
       <c r="A123">
         <v>223</v>
       </c>
       <c r="B123" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C123" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D123" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E123" t="b">
         <v>0</v>
@@ -3745,19 +4198,22 @@
       <c r="H123" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:8">
+      <c r="I123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
       <c r="A124">
         <v>236</v>
       </c>
       <c r="B124" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C124" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D124" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="E124" t="b">
         <v>0</v>
@@ -3771,19 +4227,22 @@
       <c r="H124" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:8">
+      <c r="I124" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
       <c r="A125">
         <v>165</v>
       </c>
       <c r="B125" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C125" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D125" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E125" t="b">
         <v>0</v>
@@ -3797,19 +4256,22 @@
       <c r="H125" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:8">
+      <c r="I125" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
       <c r="A126">
         <v>206</v>
       </c>
       <c r="B126" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C126" t="s">
-        <v>17</v>
-      </c>
-      <c r="D126">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="D126" t="s">
+        <v>24</v>
       </c>
       <c r="E126" t="b">
         <v>0</v>
@@ -3821,21 +4283,24 @@
         <v>0</v>
       </c>
       <c r="H126" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I126" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
       <c r="A127">
         <v>214</v>
       </c>
       <c r="B127" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C127" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D127" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="E127" t="b">
         <v>0</v>
@@ -3849,19 +4314,22 @@
       <c r="H127" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:8">
+      <c r="I127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
       <c r="A128">
         <v>230</v>
       </c>
       <c r="B128" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C128" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D128" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="E128" t="b">
         <v>0</v>
@@ -3875,19 +4343,22 @@
       <c r="H128" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:8">
+      <c r="I128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
       <c r="A129">
         <v>238</v>
       </c>
       <c r="B129" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C129" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D129" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="E129" t="b">
         <v>0</v>
@@ -3901,16 +4372,22 @@
       <c r="H129" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:8">
+      <c r="I129" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
       <c r="A130">
         <v>175</v>
       </c>
       <c r="B130" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C130" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D130" t="s">
+        <v>41</v>
       </c>
       <c r="E130" t="b">
         <v>1</v>
@@ -3922,21 +4399,24 @@
         <v>0</v>
       </c>
       <c r="H130" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I130" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
       <c r="A131">
         <v>209</v>
       </c>
       <c r="B131" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C131" t="s">
-        <v>18</v>
-      </c>
-      <c r="D131">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="D131" t="s">
+        <v>73</v>
       </c>
       <c r="E131" t="b">
         <v>0</v>
@@ -3950,19 +4430,22 @@
       <c r="H131" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:8">
+      <c r="I131" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
       <c r="A132">
         <v>222</v>
       </c>
       <c r="B132" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C132" t="s">
-        <v>18</v>
-      </c>
-      <c r="D132">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="D132" t="s">
+        <v>73</v>
       </c>
       <c r="E132" t="b">
         <v>0</v>
@@ -3976,19 +4459,22 @@
       <c r="H132" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:8">
+      <c r="I132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
       <c r="A133">
         <v>223</v>
       </c>
       <c r="B133" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C133" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D133" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E133" t="b">
         <v>0</v>
@@ -4002,19 +4488,22 @@
       <c r="H133" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:8">
+      <c r="I133" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
       <c r="A134">
         <v>236</v>
       </c>
       <c r="B134" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C134" t="s">
-        <v>18</v>
-      </c>
-      <c r="D134">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="D134" t="s">
+        <v>22</v>
       </c>
       <c r="E134" t="b">
         <v>0</v>
@@ -4028,19 +4517,22 @@
       <c r="H134" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:8">
+      <c r="I134" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9">
       <c r="A135">
         <v>182</v>
       </c>
       <c r="B135" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C135" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D135" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E135" t="b">
         <v>0</v>
@@ -4054,19 +4546,22 @@
       <c r="H135" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:8">
+      <c r="I135" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
       <c r="A136">
         <v>210</v>
       </c>
       <c r="B136" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C136" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D136" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E136" t="b">
         <v>0</v>
@@ -4080,16 +4575,22 @@
       <c r="H136" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:8">
+      <c r="I136" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9">
       <c r="A137">
         <v>212</v>
       </c>
       <c r="B137" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C137" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D137" t="s">
+        <v>41</v>
       </c>
       <c r="E137" t="b">
         <v>1</v>
@@ -4101,18 +4602,24 @@
         <v>0</v>
       </c>
       <c r="H137" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I137" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9">
       <c r="A138">
         <v>226</v>
       </c>
       <c r="B138" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C138" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D138" t="s">
+        <v>41</v>
       </c>
       <c r="E138" t="b">
         <v>1</v>
@@ -4124,21 +4631,24 @@
         <v>0</v>
       </c>
       <c r="H138" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I138" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9">
       <c r="A139">
         <v>234</v>
       </c>
       <c r="B139" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C139" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D139" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="E139" t="b">
         <v>0</v>
@@ -4152,19 +4662,22 @@
       <c r="H139" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:8">
+      <c r="I139" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9">
       <c r="A140">
         <v>198</v>
       </c>
       <c r="B140" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C140" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D140" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E140" t="b">
         <v>0</v>
@@ -4178,19 +4691,22 @@
       <c r="H140" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:8">
+      <c r="I140" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9">
       <c r="A141">
         <v>211</v>
       </c>
       <c r="B141" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C141" t="s">
-        <v>18</v>
-      </c>
-      <c r="D141">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="D141" t="s">
+        <v>24</v>
       </c>
       <c r="E141" t="b">
         <v>0</v>
@@ -4204,19 +4720,22 @@
       <c r="H141" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:8">
+      <c r="I141" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9">
       <c r="A142">
         <v>224</v>
       </c>
       <c r="B142" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C142" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D142" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="E142" t="b">
         <v>0</v>
@@ -4230,16 +4749,22 @@
       <c r="H142" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:8">
+      <c r="I142" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9">
       <c r="A143">
         <v>231</v>
       </c>
       <c r="B143" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C143" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D143" t="s">
+        <v>41</v>
       </c>
       <c r="E143" t="b">
         <v>1</v>
@@ -4251,18 +4776,24 @@
         <v>0</v>
       </c>
       <c r="H143" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I143" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9">
       <c r="A144">
         <v>232</v>
       </c>
       <c r="B144" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C144" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D144" t="s">
+        <v>41</v>
       </c>
       <c r="E144" t="b">
         <v>1</v>
@@ -4274,18 +4805,24 @@
         <v>0</v>
       </c>
       <c r="H144" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I144" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9">
       <c r="A145">
         <v>235</v>
       </c>
       <c r="B145" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C145" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D145" t="s">
+        <v>41</v>
       </c>
       <c r="E145" t="b">
         <v>0</v>
@@ -4299,19 +4836,22 @@
       <c r="H145" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:8">
+      <c r="I145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9">
       <c r="A146">
         <v>240</v>
       </c>
       <c r="B146" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C146" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D146" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="E146" t="b">
         <v>0</v>
@@ -4325,19 +4865,22 @@
       <c r="H146" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:8">
+      <c r="I146" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9">
       <c r="A147">
         <v>175</v>
       </c>
       <c r="B147" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C147" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D147" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E147" t="b">
         <v>0</v>
@@ -4351,19 +4894,22 @@
       <c r="H147" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:8">
+      <c r="I147" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9">
       <c r="A148">
         <v>209</v>
       </c>
       <c r="B148" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C148" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D148" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="E148" t="b">
         <v>0</v>
@@ -4377,19 +4923,22 @@
       <c r="H148" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:8">
+      <c r="I148" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9">
       <c r="A149">
         <v>222</v>
       </c>
       <c r="B149" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C149" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D149" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E149" t="b">
         <v>0</v>
@@ -4403,19 +4952,22 @@
       <c r="H149" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:8">
+      <c r="I149" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9">
       <c r="A150">
         <v>223</v>
       </c>
       <c r="B150" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C150" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D150" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="E150" t="b">
         <v>0</v>
@@ -4429,19 +4981,22 @@
       <c r="H150" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:8">
+      <c r="I150" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9">
       <c r="A151">
         <v>236</v>
       </c>
       <c r="B151" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C151" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D151" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="E151" t="b">
         <v>0</v>
@@ -4455,19 +5010,22 @@
       <c r="H151" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:8">
+      <c r="I151" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9">
       <c r="A152">
         <v>198</v>
       </c>
       <c r="B152" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C152" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D152" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E152" t="b">
         <v>0</v>
@@ -4481,19 +5039,22 @@
       <c r="H152" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:8">
+      <c r="I152" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9">
       <c r="A153">
         <v>211</v>
       </c>
       <c r="B153" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C153" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D153" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E153" t="b">
         <v>0</v>
@@ -4507,19 +5068,22 @@
       <c r="H153" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:8">
+      <c r="I153" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9">
       <c r="A154">
         <v>182</v>
       </c>
       <c r="B154" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C154" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D154" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E154" t="b">
         <v>0</v>
@@ -4533,19 +5097,22 @@
       <c r="H154" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:8">
+      <c r="I154" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9">
       <c r="A155">
         <v>210</v>
       </c>
       <c r="B155" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C155" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D155" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="E155" t="b">
         <v>0</v>
@@ -4559,19 +5126,22 @@
       <c r="H155" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:8">
+      <c r="I155" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9">
       <c r="A156">
         <v>212</v>
       </c>
       <c r="B156" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C156" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D156" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="E156" t="b">
         <v>0</v>
@@ -4585,19 +5155,22 @@
       <c r="H156" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:8">
+      <c r="I156" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9">
       <c r="A157">
         <v>226</v>
       </c>
       <c r="B157" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C157" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D157" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="E157" t="b">
         <v>0</v>
@@ -4611,19 +5184,22 @@
       <c r="H157" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:8">
+      <c r="I157" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9">
       <c r="A158">
         <v>234</v>
       </c>
       <c r="B158" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C158" t="s">
-        <v>19</v>
-      </c>
-      <c r="D158">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="D158" t="s">
+        <v>85</v>
       </c>
       <c r="E158" t="b">
         <v>0</v>
@@ -4635,6 +5211,9 @@
         <v>0</v>
       </c>
       <c r="H158" t="b">
+        <v>0</v>
+      </c>
+      <c r="I158" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>